<commit_message>
Remove UF features at origin from combine files and model scripts
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/dist_commute/Berlin.xlsx
+++ b/outputs/ML_Results/dist_commute/Berlin.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ24888199" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ25454087" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="summ26031112" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ26562259" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ27110166" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ27645367" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ28178018" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ28745745" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ29306033" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ24020574" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ24568600" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ25145909" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="summ25717276" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ26289610" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ26894081" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ27573131" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ28157992" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ28816908" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,10 +466,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8171.934062794435</v>
+        <v>8178.772395027099</v>
       </c>
       <c r="C2" t="n">
-        <v>8.807866354448987e-23</v>
+        <v>8.203531870268398e-23</v>
       </c>
     </row>
     <row r="3">
@@ -479,10 +479,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-642.0397931703455</v>
+        <v>-641.9834718432111</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1067501793831945</v>
+        <v>0.1067796485152576</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-203.1227719754688</v>
+        <v>-203.2017797549923</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5251749849218181</v>
+        <v>0.5250057696982646</v>
       </c>
     </row>
     <row r="5">
@@ -505,10 +505,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>39.26628374153327</v>
+        <v>40.23942052609073</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7766520992275718</v>
+        <v>0.771266364009179</v>
       </c>
     </row>
     <row r="6">
@@ -518,10 +518,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-112.6316342999378</v>
+        <v>-112.8103189182527</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4378118325225664</v>
+        <v>0.4370849987905434</v>
       </c>
     </row>
     <row r="7">
@@ -531,10 +531,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.31849767045729</v>
+        <v>2.567493815263134</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9835044291544768</v>
+        <v>0.9872371171078341</v>
       </c>
     </row>
     <row r="8">
@@ -544,10 +544,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>62.56240219662466</v>
+        <v>62.47927028061913</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6679286042538914</v>
+        <v>0.6683421316482134</v>
       </c>
     </row>
     <row r="9">
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-66.74178059202305</v>
+        <v>-66.64805026230627</v>
       </c>
       <c r="C9" t="n">
-        <v>0.168685360335971</v>
+        <v>0.1692206402031637</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1328.105929706257</v>
+        <v>-1328.027541905499</v>
       </c>
       <c r="C10" t="n">
-        <v>5.049587488654682e-34</v>
+        <v>5.08858224795884e-34</v>
       </c>
     </row>
     <row r="11">
@@ -583,10 +583,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-25.06894365678354</v>
+        <v>-25.14323686128788</v>
       </c>
       <c r="C11" t="n">
-        <v>8.06443596569204e-07</v>
+        <v>7.639842666617522e-07</v>
       </c>
     </row>
     <row r="12">
@@ -596,10 +596,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>73.04807748428664</v>
+        <v>74.18995526414943</v>
       </c>
       <c r="C12" t="n">
-        <v>0.05821072832177777</v>
+        <v>0.05305339588308229</v>
       </c>
     </row>
     <row r="13">
@@ -609,10 +609,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>650.6954234312087</v>
+        <v>650.3166602870095</v>
       </c>
       <c r="C13" t="n">
-        <v>2.581474163163029e-194</v>
+        <v>1.092953688222397e-193</v>
       </c>
     </row>
     <row r="14">
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.02889831145733529</v>
+        <v>-0.02540088777143187</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1453159700782284</v>
+        <v>0.134239427886842</v>
       </c>
     </row>
     <row r="15">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.870479004479188e-05</v>
+        <v>-1.770604662159476e-05</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5501979411772018</v>
+        <v>0.5729683286793446</v>
       </c>
     </row>
     <row r="16">
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-15.38978158082429</v>
+        <v>-15.42875571452888</v>
       </c>
       <c r="C16" t="n">
-        <v>0.04543128986465877</v>
+        <v>0.04483094129181924</v>
       </c>
     </row>
     <row r="17">
@@ -661,10 +661,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-7.31495239669586</v>
+        <v>-7.386588607517933</v>
       </c>
       <c r="C17" t="n">
-        <v>0.05892816784362136</v>
+        <v>0.05632517856021817</v>
       </c>
     </row>
     <row r="18">
@@ -674,10 +674,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-143.0231807994014</v>
+        <v>-109.0164700918131</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8497273894873243</v>
+        <v>0.8832654371557267</v>
       </c>
     </row>
     <row r="19">
@@ -687,10 +687,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>34.32618894777636</v>
+        <v>32.16936758957354</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9373316379596377</v>
+        <v>0.9411149934755557</v>
       </c>
     </row>
   </sheetData>
@@ -736,10 +736,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8307.043385717279</v>
+        <v>8323.897808068523</v>
       </c>
       <c r="C2" t="n">
-        <v>3.334011606049253e-23</v>
+        <v>2.752088678988473e-23</v>
       </c>
     </row>
     <row r="3">
@@ -749,10 +749,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-372.1390114694955</v>
+        <v>-372.0614335014359</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3549974379313355</v>
+        <v>0.3550939250129226</v>
       </c>
     </row>
     <row r="4">
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-292.2298336423212</v>
+        <v>-292.9818223346705</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3538796098904927</v>
+        <v>0.3526426123096673</v>
       </c>
     </row>
     <row r="5">
@@ -775,10 +775,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-16.77400972673858</v>
+        <v>-16.41507723391487</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9028315773457546</v>
+        <v>0.9048998100328873</v>
       </c>
     </row>
     <row r="6">
@@ -788,10 +788,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>64.71953120103655</v>
+        <v>64.49095051162641</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6532897112315619</v>
+        <v>0.6544341649932366</v>
       </c>
     </row>
     <row r="7">
@@ -801,10 +801,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>37.45143934207057</v>
+        <v>37.19340547525994</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8143405101844798</v>
+        <v>0.8155943974183699</v>
       </c>
     </row>
     <row r="8">
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>176.8713823304973</v>
+        <v>176.8331672008806</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2239286682183913</v>
+        <v>0.2240258020051572</v>
       </c>
     </row>
     <row r="9">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-34.50168580743043</v>
+        <v>-34.66586805273019</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4740227245351046</v>
+        <v>0.4718542804513868</v>
       </c>
     </row>
     <row r="10">
@@ -840,10 +840,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1327.198761184977</v>
+        <v>-1327.114082967366</v>
       </c>
       <c r="C10" t="n">
-        <v>2.748815058871498e-34</v>
+        <v>2.762332336365539e-34</v>
       </c>
     </row>
     <row r="11">
@@ -853,10 +853,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-21.79437211883694</v>
+        <v>-21.89766012432628</v>
       </c>
       <c r="C11" t="n">
-        <v>1.776286771929829e-05</v>
+        <v>1.645119448919087e-05</v>
       </c>
     </row>
     <row r="12">
@@ -866,10 +866,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>111.7221198902064</v>
+        <v>111.9453941316421</v>
       </c>
       <c r="C12" t="n">
-        <v>0.003466406330175585</v>
+        <v>0.003222906942139999</v>
       </c>
     </row>
     <row r="13">
@@ -879,10 +879,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>651.1446070743056</v>
+        <v>650.4224370559476</v>
       </c>
       <c r="C13" t="n">
-        <v>2.781826536503388e-195</v>
+        <v>1.831545828172513e-194</v>
       </c>
     </row>
     <row r="14">
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.01942134828255922</v>
+        <v>-0.01834974268337124</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3260925579203476</v>
+        <v>0.2775578955169751</v>
       </c>
     </row>
     <row r="15">
@@ -905,10 +905,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-2.165094720704854e-05</v>
+        <v>-1.964192475467655e-05</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4938636397082475</v>
+        <v>0.5360248199699753</v>
       </c>
     </row>
     <row r="16">
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-23.315026696779</v>
+        <v>-23.31231546665168</v>
       </c>
       <c r="C16" t="n">
-        <v>0.002285123643071629</v>
+        <v>0.002284060785789463</v>
       </c>
     </row>
     <row r="17">
@@ -931,10 +931,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-9.89196900133561</v>
+        <v>-9.93567221195962</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01105942655240676</v>
+        <v>0.0106670613702506</v>
       </c>
     </row>
     <row r="18">
@@ -944,10 +944,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>313.4449203911363</v>
+        <v>314.9202021317424</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6785414425694066</v>
+        <v>0.6718745805881288</v>
       </c>
     </row>
     <row r="19">
@@ -957,10 +957,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.289781865412806</v>
+        <v>8.741919144748863</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9957878099183832</v>
+        <v>0.9838806093071091</v>
       </c>
     </row>
   </sheetData>
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8419.054269369244</v>
+        <v>8395.73589617429</v>
       </c>
       <c r="C2" t="n">
-        <v>3.133438455125496e-24</v>
+        <v>4.200895725738224e-24</v>
       </c>
     </row>
     <row r="3">
@@ -1019,10 +1019,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-516.6556566999341</v>
+        <v>-517.1048508792494</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1932748640678528</v>
+        <v>0.1928971513830822</v>
       </c>
     </row>
     <row r="4">
@@ -1032,10 +1032,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-322.7172955086176</v>
+        <v>-321.7618676527944</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3118361242754886</v>
+        <v>0.3132811562835688</v>
       </c>
     </row>
     <row r="5">
@@ -1045,10 +1045,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>81.15013964083693</v>
+        <v>82.2014875827914</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5544738016075086</v>
+        <v>0.5493568014145775</v>
       </c>
     </row>
     <row r="6">
@@ -1058,10 +1058,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-83.8747486373239</v>
+        <v>-83.4319215292098</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5597530761152615</v>
+        <v>0.5618320207821592</v>
       </c>
     </row>
     <row r="7">
@@ -1071,10 +1071,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-123.771687259455</v>
+        <v>-124.6020795200708</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4360776513493833</v>
+        <v>0.4330146246819644</v>
       </c>
     </row>
     <row r="8">
@@ -1084,10 +1084,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-12.00797945367012</v>
+        <v>-12.029523738932</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9341903885698095</v>
+        <v>0.9340738441210027</v>
       </c>
     </row>
     <row r="9">
@@ -1097,10 +1097,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-23.8504837049048</v>
+        <v>-23.15822476067385</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6190428108305399</v>
+        <v>0.6292066661713039</v>
       </c>
     </row>
     <row r="10">
@@ -1110,10 +1110,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1338.473618527528</v>
+        <v>-1338.062923771486</v>
       </c>
       <c r="C10" t="n">
-        <v>5.227055741804322e-35</v>
+        <v>5.488981100945229e-35</v>
       </c>
     </row>
     <row r="11">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-24.20670887792534</v>
+        <v>-24.14175587536019</v>
       </c>
       <c r="C11" t="n">
-        <v>1.856558903388581e-06</v>
+        <v>2.008918601345627e-06</v>
       </c>
     </row>
     <row r="12">
@@ -1136,10 +1136,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>84.27945990446096</v>
+        <v>87.57822774715264</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02783454821065711</v>
+        <v>0.0215202950237715</v>
       </c>
     </row>
     <row r="13">
@@ -1149,10 +1149,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>657.0374746401753</v>
+        <v>657.9004447239836</v>
       </c>
       <c r="C13" t="n">
-        <v>6.818626281708279e-200</v>
+        <v>4.904963437468352e-200</v>
       </c>
     </row>
     <row r="14">
@@ -1162,10 +1162,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.04013712072897864</v>
+        <v>-0.03159239509602171</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04029533069275905</v>
+        <v>0.05846489650426721</v>
       </c>
     </row>
     <row r="15">
@@ -1175,10 +1175,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3.973460616875097e-06</v>
+        <v>1.59335285431251e-06</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8974414567715001</v>
+        <v>0.9588871779376786</v>
       </c>
     </row>
     <row r="16">
@@ -1188,10 +1188,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-20.60680057057144</v>
+        <v>-20.74282467682293</v>
       </c>
       <c r="C16" t="n">
-        <v>0.007057231837255588</v>
+        <v>0.006676883911341705</v>
       </c>
     </row>
     <row r="17">
@@ -1201,10 +1201,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-9.539313837975133</v>
+        <v>-9.680840996616581</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01297720302126795</v>
+        <v>0.01163605626032606</v>
       </c>
     </row>
     <row r="18">
@@ -1214,10 +1214,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-438.205207260808</v>
+        <v>-329.151288838354</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5577771075081754</v>
+        <v>0.6543162721762897</v>
       </c>
     </row>
     <row r="19">
@@ -1227,10 +1227,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>111.8533583521482</v>
+        <v>86.42410781280387</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7968365537073372</v>
+        <v>0.8419520750205012</v>
       </c>
     </row>
   </sheetData>
@@ -1276,10 +1276,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7728.644659673484</v>
+        <v>7726.827875265241</v>
       </c>
       <c r="C2" t="n">
-        <v>1.41589421299258e-20</v>
+        <v>1.4741916091868e-20</v>
       </c>
     </row>
     <row r="3">
@@ -1289,10 +1289,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-600.8615349572838</v>
+        <v>-600.4187489483004</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1311580863611746</v>
+        <v>0.1314426899523374</v>
       </c>
     </row>
     <row r="4">
@@ -1302,10 +1302,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-528.6921193921323</v>
+        <v>-529.2273212496325</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09401621344660568</v>
+        <v>0.09369409625721492</v>
       </c>
     </row>
     <row r="5">
@@ -1315,10 +1315,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>62.48898361659739</v>
+        <v>63.01377770202942</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6500019468970142</v>
+        <v>0.6472550144936653</v>
       </c>
     </row>
     <row r="6">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24.94918631153194</v>
+        <v>25.09494912117033</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8627652345260554</v>
+        <v>0.8619713775027211</v>
       </c>
     </row>
     <row r="7">
@@ -1341,10 +1341,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-40.49825393686888</v>
+        <v>-40.82892099273766</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7995325941819054</v>
+        <v>0.7979313379698098</v>
       </c>
     </row>
     <row r="8">
@@ -1354,10 +1354,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>26.36885474381558</v>
+        <v>26.38458867047684</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8556195038965325</v>
+        <v>0.8555346165285751</v>
       </c>
     </row>
     <row r="9">
@@ -1367,10 +1367,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-40.45055580917622</v>
+        <v>-40.04904491766108</v>
       </c>
       <c r="C9" t="n">
-        <v>0.401565593378759</v>
+        <v>0.4061429119037081</v>
       </c>
     </row>
     <row r="10">
@@ -1380,10 +1380,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1229.207749920574</v>
+        <v>-1228.884915599072</v>
       </c>
       <c r="C10" t="n">
-        <v>1.111156334037949e-29</v>
+        <v>1.147575647125304e-29</v>
       </c>
     </row>
     <row r="11">
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-18.60406759170471</v>
+        <v>-18.63413484691683</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0002450532076821222</v>
+        <v>0.0002422047914409224</v>
       </c>
     </row>
     <row r="12">
@@ -1406,10 +1406,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>69.5960333822772</v>
+        <v>71.44677734078851</v>
       </c>
       <c r="C12" t="n">
-        <v>0.06949233371636195</v>
+        <v>0.06092579994190287</v>
       </c>
     </row>
     <row r="13">
@@ -1419,10 +1419,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>656.8128217334928</v>
+        <v>656.80840112063</v>
       </c>
       <c r="C13" t="n">
-        <v>8.690516221694287e-198</v>
+        <v>2.512431295970521e-197</v>
       </c>
     </row>
     <row r="14">
@@ -1432,10 +1432,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.03249636667834034</v>
+        <v>-0.02736291840327242</v>
       </c>
       <c r="C14" t="n">
-        <v>0.09912230800498956</v>
+        <v>0.103877344855684</v>
       </c>
     </row>
     <row r="15">
@@ -1445,10 +1445,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>9.137520569494999e-06</v>
+        <v>9.023789246325566e-06</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7696741925715853</v>
+        <v>0.773128561176483</v>
       </c>
     </row>
     <row r="16">
@@ -1458,10 +1458,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-17.25304083586812</v>
+        <v>-17.32696780771187</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02382236120065977</v>
+        <v>0.02318842306028679</v>
       </c>
     </row>
     <row r="17">
@@ -1471,10 +1471,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-6.744890775413509</v>
+        <v>-6.843271283759769</v>
       </c>
       <c r="C17" t="n">
-        <v>0.08007022395268672</v>
+        <v>0.07557529463744669</v>
       </c>
     </row>
     <row r="18">
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-462.5964516701861</v>
+        <v>-406.1479873698308</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5371152171467068</v>
+        <v>0.5818214323233528</v>
       </c>
     </row>
     <row r="19">
@@ -1497,10 +1497,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-176.6145978172501</v>
+        <v>-186.2425962987745</v>
       </c>
       <c r="C19" t="n">
-        <v>0.683687952152722</v>
+        <v>0.6666797733689764</v>
       </c>
     </row>
   </sheetData>
@@ -1546,10 +1546,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7338.158854236305</v>
+        <v>7364.833868822603</v>
       </c>
       <c r="C2" t="n">
-        <v>1.611669786872342e-18</v>
+        <v>1.218241449463349e-18</v>
       </c>
     </row>
     <row r="3">
@@ -1559,10 +1559,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-652.1671788881564</v>
+        <v>-652.5100457416922</v>
       </c>
       <c r="C3" t="n">
-        <v>0.105726112408938</v>
+        <v>0.1055359189303735</v>
       </c>
     </row>
     <row r="4">
@@ -1572,10 +1572,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-204.4759604872617</v>
+        <v>-206.2912802255298</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5176029666271771</v>
+        <v>0.513892635524182</v>
       </c>
     </row>
     <row r="5">
@@ -1585,10 +1585,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>64.72360119737506</v>
+        <v>65.59718574485362</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6387028655092286</v>
+        <v>0.6341631057752883</v>
       </c>
     </row>
     <row r="6">
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>91.19554469363078</v>
+        <v>91.12730784731582</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5290397657242816</v>
+        <v>0.5293393893776354</v>
       </c>
     </row>
     <row r="7">
@@ -1611,10 +1611,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>102.5785371156822</v>
+        <v>102.0015868703839</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5233281534345591</v>
+        <v>0.5256589717081765</v>
       </c>
     </row>
     <row r="8">
@@ -1624,10 +1624,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>104.0688976467908</v>
+        <v>104.1145515362066</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4767675179963349</v>
+        <v>0.4765651100537055</v>
       </c>
     </row>
     <row r="9">
@@ -1637,10 +1637,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-84.84013323354672</v>
+        <v>-85.13932428312327</v>
       </c>
       <c r="C9" t="n">
-        <v>0.08099272083156846</v>
+        <v>0.07987078514193979</v>
       </c>
     </row>
     <row r="10">
@@ -1650,10 +1650,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1178.508720440936</v>
+        <v>-1178.341917384726</v>
       </c>
       <c r="C10" t="n">
-        <v>4.276905536936132e-27</v>
+        <v>4.332002146302962e-27</v>
       </c>
     </row>
     <row r="11">
@@ -1663,10 +1663,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-25.75160861670666</v>
+        <v>-25.92873736473189</v>
       </c>
       <c r="C11" t="n">
-        <v>4.247393547453561e-07</v>
+        <v>3.604985753333723e-07</v>
       </c>
     </row>
     <row r="12">
@@ -1676,10 +1676,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>90.09027949487904</v>
+        <v>90.55442060363532</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01843579638195939</v>
+        <v>0.01723644672737644</v>
       </c>
     </row>
     <row r="13">
@@ -1689,10 +1689,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>639.5423332186783</v>
+        <v>638.3523318933479</v>
       </c>
       <c r="C13" t="n">
-        <v>8.277125807750217e-188</v>
+        <v>7.121139719283936e-187</v>
       </c>
     </row>
     <row r="14">
@@ -1702,10 +1702,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.03558191654299425</v>
+        <v>-0.03340407465426239</v>
       </c>
       <c r="C14" t="n">
-        <v>0.07409870386853493</v>
+        <v>0.04951939828238095</v>
       </c>
     </row>
     <row r="15">
@@ -1715,10 +1715,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.125671077147663e-05</v>
+        <v>-7.709063682944274e-06</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7232515736872673</v>
+        <v>0.8090103216402731</v>
       </c>
     </row>
     <row r="16">
@@ -1728,10 +1728,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-12.82484845034787</v>
+        <v>-12.80668311252496</v>
       </c>
       <c r="C16" t="n">
-        <v>0.09751010746763551</v>
+        <v>0.09790062191430809</v>
       </c>
     </row>
     <row r="17">
@@ -1741,10 +1741,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-2.57411525063424</v>
+        <v>-2.648017360400139</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5083047199628035</v>
+        <v>0.495884691156004</v>
       </c>
     </row>
     <row r="18">
@@ -1754,10 +1754,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-96.59678342334701</v>
+        <v>-91.21020581645098</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8979548007576024</v>
+        <v>0.9020368997147262</v>
       </c>
     </row>
     <row r="19">
@@ -1767,10 +1767,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>253.4450805255331</v>
+        <v>263.4005663311268</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5611870102735925</v>
+        <v>0.5448577121695661</v>
       </c>
     </row>
   </sheetData>
@@ -1816,10 +1816,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8083.179097214762</v>
+        <v>8102.362633832112</v>
       </c>
       <c r="C2" t="n">
-        <v>2.620984961939359e-22</v>
+        <v>2.121043935479336e-22</v>
       </c>
     </row>
     <row r="3">
@@ -1829,10 +1829,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-306.2290965591461</v>
+        <v>-305.9098828492993</v>
       </c>
       <c r="C3" t="n">
-        <v>0.450917004143618</v>
+        <v>0.4513868202660402</v>
       </c>
     </row>
     <row r="4">
@@ -1842,10 +1842,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>114.0149188525091</v>
+        <v>113.3109927171392</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7212459594472396</v>
+        <v>0.7228930144481829</v>
       </c>
     </row>
     <row r="5">
@@ -1855,10 +1855,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>73.78277498581008</v>
+        <v>74.13032911674196</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5918321600861438</v>
+        <v>0.5900825672845076</v>
       </c>
     </row>
     <row r="6">
@@ -1868,10 +1868,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-24.44813239810968</v>
+        <v>-24.45914820512148</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8664035138143856</v>
+        <v>0.8663428165437984</v>
       </c>
     </row>
     <row r="7">
@@ -1881,10 +1881,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46.72533938430794</v>
+        <v>46.68744813907972</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7719683484970939</v>
+        <v>0.7721458686598193</v>
       </c>
     </row>
     <row r="8">
@@ -1894,10 +1894,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>100.1912716717796</v>
+        <v>100.2818513043581</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4933805886260146</v>
+        <v>0.4929870323190569</v>
       </c>
     </row>
     <row r="9">
@@ -1907,10 +1907,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-65.43105794864027</v>
+        <v>-65.68196301511203</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1780930763935992</v>
+        <v>0.1763432722129444</v>
       </c>
     </row>
     <row r="10">
@@ -1920,10 +1920,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1360.616152131323</v>
+        <v>-1360.519689186247</v>
       </c>
       <c r="C10" t="n">
-        <v>2.029462180566388e-35</v>
+        <v>2.049747314905113e-35</v>
       </c>
     </row>
     <row r="11">
@@ -1933,10 +1933,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-23.63562329584926</v>
+        <v>-23.75145658495695</v>
       </c>
       <c r="C11" t="n">
-        <v>3.969310493237059e-06</v>
+        <v>3.63400729052899e-06</v>
       </c>
     </row>
     <row r="12">
@@ -1946,10 +1946,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>72.91328852127043</v>
+        <v>72.79773010520842</v>
       </c>
       <c r="C12" t="n">
-        <v>0.05684106764163201</v>
+        <v>0.05583731086580133</v>
       </c>
     </row>
     <row r="13">
@@ -1959,10 +1959,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>671.8983394768113</v>
+        <v>671.065968030334</v>
       </c>
       <c r="C13" t="n">
-        <v>7.185788400130627e-205</v>
+        <v>6.056609727476304e-204</v>
       </c>
     </row>
     <row r="14">
@@ -1972,10 +1972,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.01559897211303356</v>
+        <v>-0.01537659527750936</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4318890717406703</v>
+        <v>0.3643792391915435</v>
       </c>
     </row>
     <row r="15">
@@ -1985,10 +1985,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-2.006395307266854e-05</v>
+        <v>-1.784391621527761e-05</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5216886378979957</v>
+        <v>0.5697850697856008</v>
       </c>
     </row>
     <row r="16">
@@ -1998,10 +1998,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-16.83662983237305</v>
+        <v>-16.81604070053336</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02887122889655788</v>
+        <v>0.02902317275509392</v>
       </c>
     </row>
     <row r="17">
@@ -2011,10 +2011,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-9.535273564195457</v>
+        <v>-9.561715209836255</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01316448884391353</v>
+        <v>0.01285406954782898</v>
       </c>
     </row>
     <row r="18">
@@ -2024,10 +2024,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>356.2254585601627</v>
+        <v>347.5657807929392</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6380191906795812</v>
+        <v>0.6405554919257657</v>
       </c>
     </row>
     <row r="19">
@@ -2037,10 +2037,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-103.6271094426054</v>
+        <v>-94.7001851244072</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8125777870835729</v>
+        <v>0.8280533320494776</v>
       </c>
     </row>
   </sheetData>
@@ -2086,10 +2086,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8623.152312800143</v>
+        <v>8622.520344304083</v>
       </c>
       <c r="C2" t="n">
-        <v>5.251371653333158e-25</v>
+        <v>5.417843050041039e-25</v>
       </c>
     </row>
     <row r="3">
@@ -2099,10 +2099,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-551.8731462091581</v>
+        <v>-551.926192101368</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1701054245810611</v>
+        <v>0.1700648368753145</v>
       </c>
     </row>
     <row r="4">
@@ -2112,10 +2112,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.734430730333543</v>
+        <v>8.697574307513264</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9778901243546525</v>
+        <v>0.9779835340134484</v>
       </c>
     </row>
     <row r="5">
@@ -2125,10 +2125,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>152.0455090560976</v>
+        <v>152.6749201891291</v>
       </c>
       <c r="C5" t="n">
-        <v>0.266239250851959</v>
+        <v>0.2642561605620293</v>
       </c>
     </row>
     <row r="6">
@@ -2138,10 +2138,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27.67564686284209</v>
+        <v>27.48871596795344</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8478190740668947</v>
+        <v>0.8488343944308604</v>
       </c>
     </row>
     <row r="7">
@@ -2151,10 +2151,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-13.42832120875229</v>
+        <v>-14.03561562186147</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9329718049272713</v>
+        <v>0.9299475617442189</v>
       </c>
     </row>
     <row r="8">
@@ -2164,10 +2164,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>73.71735081751521</v>
+        <v>73.55797996332697</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6121399869305452</v>
+        <v>0.6129087006159046</v>
       </c>
     </row>
     <row r="9">
@@ -2177,10 +2177,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-26.16749437781162</v>
+        <v>-25.98626522141861</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5883572190277686</v>
+        <v>0.590894798437102</v>
       </c>
     </row>
     <row r="10">
@@ -2190,10 +2190,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1293.716505835313</v>
+        <v>-1293.451835993735</v>
       </c>
       <c r="C10" t="n">
-        <v>1.193035309795364e-32</v>
+        <v>1.226281269637663e-32</v>
       </c>
     </row>
     <row r="11">
@@ -2203,10 +2203,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-23.1630201668919</v>
+        <v>-23.19425511222323</v>
       </c>
       <c r="C11" t="n">
-        <v>5.284820398170874e-06</v>
+        <v>5.224756975453174e-06</v>
       </c>
     </row>
     <row r="12">
@@ -2216,10 +2216,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>99.30105233064745</v>
+        <v>100.7612096803931</v>
       </c>
       <c r="C12" t="n">
-        <v>0.008975093773776067</v>
+        <v>0.007674710727906961</v>
       </c>
     </row>
     <row r="13">
@@ -2229,10 +2229,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>662.0218170755567</v>
+        <v>662.0124168008587</v>
       </c>
       <c r="C13" t="n">
-        <v>2.952924662481435e-202</v>
+        <v>6.278787323768872e-202</v>
       </c>
     </row>
     <row r="14">
@@ -2242,10 +2242,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.02731177844342783</v>
+        <v>-0.02310819474489625</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1711258094847465</v>
+        <v>0.1752208435258837</v>
       </c>
     </row>
     <row r="15">
@@ -2255,10 +2255,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-9.905964191799421e-06</v>
+        <v>-9.883183027626885e-06</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7564724984480571</v>
+        <v>0.7578051561651558</v>
       </c>
     </row>
     <row r="16">
@@ -2268,10 +2268,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-22.75537101226097</v>
+        <v>-22.81482342172613</v>
       </c>
       <c r="C16" t="n">
-        <v>0.003064252805885974</v>
+        <v>0.00298116020142572</v>
       </c>
     </row>
     <row r="17">
@@ -2281,10 +2281,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-14.03315634102001</v>
+        <v>-14.11381533121496</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0002954629447181561</v>
+        <v>0.0002704547085140748</v>
       </c>
     </row>
     <row r="18">
@@ -2294,10 +2294,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>427.1517790459802</v>
+        <v>474.1696064921571</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5721848383834396</v>
+        <v>0.5236989249482324</v>
       </c>
     </row>
     <row r="19">
@@ -2307,10 +2307,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>180.8753973651013</v>
+        <v>173.4455079786612</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6756248461261445</v>
+        <v>0.6874841029741464</v>
       </c>
     </row>
   </sheetData>
@@ -2356,10 +2356,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8215.414710940282</v>
+        <v>8216.353130142877</v>
       </c>
       <c r="C2" t="n">
-        <v>2.748425088579677e-23</v>
+        <v>2.718295559883529e-23</v>
       </c>
     </row>
     <row r="3">
@@ -2369,10 +2369,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-536.8191348345391</v>
+        <v>-537.3109968520348</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1967328684527111</v>
+        <v>0.1963238488784874</v>
       </c>
     </row>
     <row r="4">
@@ -2382,10 +2382,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-347.4781317684481</v>
+        <v>-347.7865192063899</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2684154445401065</v>
+        <v>0.2679978626677078</v>
       </c>
     </row>
     <row r="5">
@@ -2395,10 +2395,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.831571521339868</v>
+        <v>2.16308857501366</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9893361884723103</v>
+        <v>0.9874060178484025</v>
       </c>
     </row>
     <row r="6">
@@ -2408,10 +2408,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-14.22604238649454</v>
+        <v>-14.26394987435994</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9214670126601936</v>
+        <v>0.921258519390616</v>
       </c>
     </row>
     <row r="7">
@@ -2421,10 +2421,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-54.65857507417161</v>
+        <v>-55.03601081066181</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7326034868536753</v>
+        <v>0.7308259923572382</v>
       </c>
     </row>
     <row r="8">
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>85.15761819372401</v>
+        <v>85.14113095140539</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5570790349429643</v>
+        <v>0.5571548878052117</v>
       </c>
     </row>
     <row r="9">
@@ -2447,10 +2447,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-48.11494271586708</v>
+        <v>-48.00455964849351</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3192405649350508</v>
+        <v>0.3202723423292771</v>
       </c>
     </row>
     <row r="10">
@@ -2460,10 +2460,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1371.229715925994</v>
+        <v>-1371.007105284357</v>
       </c>
       <c r="C10" t="n">
-        <v>1.707444555220865e-36</v>
+        <v>1.748522444439777e-36</v>
       </c>
     </row>
     <row r="11">
@@ -2473,10 +2473,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-24.07073080416978</v>
+        <v>-24.10430832355978</v>
       </c>
       <c r="C11" t="n">
-        <v>2.015026781845449e-06</v>
+        <v>1.985464492040626e-06</v>
       </c>
     </row>
     <row r="12">
@@ -2486,10 +2486,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>115.8503089309394</v>
+        <v>116.9099676225085</v>
       </c>
       <c r="C12" t="n">
-        <v>0.002332064559072641</v>
+        <v>0.002005200597948581</v>
       </c>
     </row>
     <row r="13">
@@ -2499,10 +2499,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>663.8598820986031</v>
+        <v>663.7327084078242</v>
       </c>
       <c r="C13" t="n">
-        <v>1.254201676542998e-204</v>
+        <v>4.070113118986249e-204</v>
       </c>
     </row>
     <row r="14">
@@ -2512,10 +2512,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.02131627537337932</v>
+        <v>-0.01828924950843056</v>
       </c>
       <c r="C14" t="n">
-        <v>0.280036284248888</v>
+        <v>0.2773460188074902</v>
       </c>
     </row>
     <row r="15">
@@ -2525,10 +2525,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7.620212919966229e-06</v>
+        <v>-7.382335305984324e-06</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8080408081718039</v>
+        <v>0.8143154029211082</v>
       </c>
     </row>
     <row r="16">
@@ -2538,10 +2538,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-18.74748312901669</v>
+        <v>-18.77369093085194</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01413953675818372</v>
+        <v>0.01398837895840358</v>
       </c>
     </row>
     <row r="17">
@@ -2551,10 +2551,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-10.17985603944635</v>
+        <v>-10.23652712370759</v>
       </c>
       <c r="C17" t="n">
-        <v>0.007569694648926965</v>
+        <v>0.007203465900822257</v>
       </c>
     </row>
     <row r="18">
@@ -2564,10 +2564,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>580.3182660727816</v>
+        <v>613.2534717332674</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4383429404487409</v>
+        <v>0.4047580115490497</v>
       </c>
     </row>
     <row r="19">
@@ -2577,10 +2577,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-90.33781159547755</v>
+        <v>-94.67359964877187</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8344570130398246</v>
+        <v>0.8261939661285238</v>
       </c>
     </row>
   </sheetData>
@@ -2626,10 +2626,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8067.715143744563</v>
+        <v>8086.189493966564</v>
       </c>
       <c r="C2" t="n">
-        <v>4.027239558326346e-22</v>
+        <v>3.279214202275371e-22</v>
       </c>
     </row>
     <row r="3">
@@ -2639,10 +2639,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-906.015621383606</v>
+        <v>-905.6174663683846</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02640092028998794</v>
+        <v>0.02646601276319411</v>
       </c>
     </row>
     <row r="4">
@@ -2652,10 +2652,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-240.6792842714269</v>
+        <v>-241.1296642465669</v>
       </c>
       <c r="C4" t="n">
-        <v>0.449043461493051</v>
+        <v>0.4481913024651119</v>
       </c>
     </row>
     <row r="5">
@@ -2665,10 +2665,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-107.1872914954463</v>
+        <v>-106.881971636377</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4372164233525039</v>
+        <v>0.4385080163674809</v>
       </c>
     </row>
     <row r="6">
@@ -2678,10 +2678,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>81.29703773937452</v>
+        <v>81.25174110292076</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5743403358877359</v>
+        <v>0.5745496781118323</v>
       </c>
     </row>
     <row r="7">
@@ -2691,10 +2691,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-17.60393214009697</v>
+        <v>-17.71913187165026</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9119968636758611</v>
+        <v>0.9114219463463867</v>
       </c>
     </row>
     <row r="8">
@@ -2704,10 +2704,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>127.1104883395576</v>
+        <v>127.2458546310765</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3827674099153409</v>
+        <v>0.382258700743192</v>
       </c>
     </row>
     <row r="9">
@@ -2717,10 +2717,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-36.51062156477829</v>
+        <v>-36.73856472909881</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4487254964559404</v>
+        <v>0.4458224580966156</v>
       </c>
     </row>
     <row r="10">
@@ -2730,10 +2730,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1296.439692640764</v>
+        <v>-1296.515054102055</v>
       </c>
       <c r="C10" t="n">
-        <v>1.203649777154697e-32</v>
+        <v>1.192386282725109e-32</v>
       </c>
     </row>
     <row r="11">
@@ -2743,10 +2743,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-27.0230578484226</v>
+        <v>-27.13470139045942</v>
       </c>
       <c r="C11" t="n">
-        <v>9.99492242731766e-08</v>
+        <v>9.046238142192647e-08</v>
       </c>
     </row>
     <row r="12">
@@ -2756,10 +2756,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>120.7645245379774</v>
+        <v>120.7484593849956</v>
       </c>
       <c r="C12" t="n">
-        <v>0.001604387947855875</v>
+        <v>0.001514326584343826</v>
       </c>
     </row>
     <row r="13">
@@ -2769,10 +2769,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>653.3264391405519</v>
+        <v>652.5197829756576</v>
       </c>
       <c r="C13" t="n">
-        <v>9.644825349964771e-194</v>
+        <v>6.930754376351835e-193</v>
       </c>
     </row>
     <row r="14">
@@ -2782,10 +2782,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.01678056998157965</v>
+        <v>-0.01639327251402022</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3985707055259393</v>
+        <v>0.3349358873807202</v>
       </c>
     </row>
     <row r="15">
@@ -2795,10 +2795,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.688489702640487e-05</v>
+        <v>-1.452462369657315e-05</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5954201914738777</v>
+        <v>0.649215905100829</v>
       </c>
     </row>
     <row r="16">
@@ -2808,10 +2808,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-15.64096347577303</v>
+        <v>-15.63164674139307</v>
       </c>
       <c r="C16" t="n">
-        <v>0.04264542857543002</v>
+        <v>0.04270797125754913</v>
       </c>
     </row>
     <row r="17">
@@ -2821,10 +2821,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-8.603608014336348</v>
+        <v>-8.633152599752876</v>
       </c>
       <c r="C17" t="n">
-        <v>0.02591593179138769</v>
+        <v>0.02531465847243268</v>
       </c>
     </row>
     <row r="18">
@@ -2834,10 +2834,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>356.6212448709889</v>
+        <v>348.7326887289219</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6365803923596043</v>
+        <v>0.6387009199513922</v>
       </c>
     </row>
     <row r="19">
@@ -2847,10 +2847,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>66.86575626515014</v>
+        <v>75.81067750237025</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8777293620607056</v>
+        <v>0.8612083404817007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>